<commit_message>
Did add color legend for sprints
</commit_message>
<xml_diff>
--- a/eval s2.xlsx
+++ b/eval s2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -27,10 +27,38 @@
     <t>Excel Worksheet Name</t>
   </si>
   <si>
+    <t>Export Summary</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
     <t>Product Owner</t>
   </si>
   <si>
-    <t>Table 1</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Product Owner</t>
+    </r>
+  </si>
+  <si>
+    <t>Scrum Master</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Scrum Master</t>
+    </r>
   </si>
   <si>
     <t>Us</t>
@@ -154,9 +182,6 @@
   </si>
   <si>
     <t>Déploiement</t>
-  </si>
-  <si>
-    <t>Scrum Master</t>
   </si>
   <si>
     <t>n°</t>
@@ -250,11 +275,11 @@
     </font>
     <font>
       <sz val="9"/>
-      <color indexed="17"/>
+      <color indexed="22"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,13 +316,130 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="20"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -414,7 +556,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -436,88 +578,181 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -541,10 +776,15 @@
       <rgbColor rgb="01eef3f4"/>
       <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
+      <rgbColor rgb="ff93c175"/>
+      <rgbColor rgb="ffffdf7f"/>
+      <rgbColor rgb="ffa1b8e1"/>
       <rgbColor rgb="ff70ad47"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffd8d8d8"/>
+      <rgbColor rgb="ffd9d9d9"/>
       <rgbColor rgb="ff595959"/>
       <rgbColor rgb="ffbfbfbf"/>
     </indexedColors>
@@ -565,9 +805,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.0787122"/>
-          <c:y val="0.0555182"/>
+          <c:y val="0.0562209"/>
           <c:w val="0.899549"/>
-          <c:h val="0.822964"/>
+          <c:h val="0.820881"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -594,7 +834,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="4"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -635,86 +875,80 @@
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:xVal>
-            <c:numRef>
-              <c:f>'Scrum Master'!$J$4:$J$14</c:f>
-              <c:numCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.500000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.500000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.500000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.500000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+            <c:numLit>
+              <c:ptCount val="11"/>
+              <c:pt idx="0">
+                <c:v>0.000000</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1.500000</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3.000000</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>3.500000</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>4.000000</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>4.500000</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>5.000000</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>5.500000</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>6.000000</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>6.500000</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>7.000000</c:v>
+              </c:pt>
+            </c:numLit>
           </c:xVal>
           <c:yVal>
-            <c:numRef>
-              <c:f>'Scrum Master'!$K$4:$K$14</c:f>
-              <c:numCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>14.000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.000000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+            <c:numLit>
+              <c:ptCount val="11"/>
+              <c:pt idx="0">
+                <c:v>14.000000</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>13.000000</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>12.000000</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>11.000000</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>10.000000</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>9.000000</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>8.000000</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>7.000000</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>6.000000</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>5.000000</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4.000000</c:v>
+              </c:pt>
+            </c:numLit>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
@@ -839,9 +1073,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.491622"/>
-          <c:y val="0.931982"/>
+          <c:y val="0.931279"/>
           <c:w val="0.126796"/>
-          <c:h val="0.0680182"/>
+          <c:h val="0.0687209"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -898,9 +1132,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>400155</xdr:colOff>
+      <xdr:colOff>400157</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>163618</xdr:rowOff>
+      <xdr:rowOff>132164</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -909,7 +1143,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1862175" y="3006724"/>
-        <a:ext cx="5408681" cy="2516295"/>
+        <a:ext cx="5408683" cy="2484841"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1115,17 +1349,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1153,10 +1387,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1404,12 +1638,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1696,7 +1930,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1724,10 +1958,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1978,73 +2212,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" style="6" customWidth="1"/>
     <col min="2" max="4" width="30.5547" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="256" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="16" customHeight="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="16" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
     <row r="3" ht="0.05" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s" s="13">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" ht="16" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="16" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="16" customHeight="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="14">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="14">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="14">
         <v>3</v>
       </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="16" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9">
-      <c r="B9" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="10"/>
+      <c r="B9" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="17"/>
+      <c r="C10" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="D10" t="s" s="19">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="10"/>
       <c r="B11" t="s" s="3">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" ht="13" customHeight="1">
+      <c r="A12" s="20"/>
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>47</v>
+        <v>6</v>
+      </c>
+      <c r="E12" s="24"/>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4"/>
+      <c r="C14" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s" s="5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
+    <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Product Owner'!R1C1" tooltip="" display="Product Owner"/>
     <hyperlink ref="D12" location="'Scrum Master'!R1C1" tooltip="" display="Scrum Master"/>
+    <hyperlink ref="D12" location="'Product Owner'!R1C1" tooltip="" display="Product Owner"/>
+    <hyperlink ref="D14" location="'Scrum Master'!R1C1" tooltip="" display="Scrum Master"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2056,258 +2379,258 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="25.3516" style="6" customWidth="1"/>
-    <col min="2" max="2" width="5.67188" style="6" customWidth="1"/>
-    <col min="3" max="3" width="5.35156" style="6" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="6" customWidth="1"/>
-    <col min="5" max="5" width="128.172" style="6" customWidth="1"/>
-    <col min="6" max="6" width="1.5" style="6" customWidth="1"/>
-    <col min="7" max="7" width="124.172" style="6" customWidth="1"/>
-    <col min="8" max="256" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="25.3516" style="25" customWidth="1"/>
+    <col min="2" max="2" width="5.67188" style="25" customWidth="1"/>
+    <col min="3" max="3" width="5.35156" style="25" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="25" customWidth="1"/>
+    <col min="5" max="5" width="128.172" style="25" customWidth="1"/>
+    <col min="6" max="6" width="1.5" style="25" customWidth="1"/>
+    <col min="7" max="7" width="124.172" style="25" customWidth="1"/>
+    <col min="8" max="256" width="8.85156" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s" s="7">
+      <c r="A1" t="s" s="26">
         <v>10</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" t="s" s="9">
+      <c r="B1" t="s" s="26">
         <v>11</v>
       </c>
+      <c r="C1" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s" s="26">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s" s="26">
+        <v>14</v>
+      </c>
+      <c r="F1" s="27"/>
+      <c r="G1" t="s" s="28">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" ht="16" customHeight="1">
-      <c r="A2" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" t="s" s="9">
-        <v>15</v>
+      <c r="A2" t="s" s="29">
+        <v>16</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" t="s" s="29">
+        <v>17</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" t="s" s="29">
+        <v>18</v>
+      </c>
+      <c r="F2" s="31"/>
+      <c r="G2" t="s" s="32">
+        <v>19</v>
       </c>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" t="s" s="7">
+      <c r="A3" t="s" s="29">
+        <v>20</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" t="s" s="29">
         <v>17</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" t="s" s="9">
-        <v>18</v>
+      <c r="D3" s="30"/>
+      <c r="E3" t="s" s="29">
+        <v>21</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" t="s" s="32">
+        <v>22</v>
       </c>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" t="s" s="9">
-        <v>21</v>
+      <c r="A4" t="s" s="29">
+        <v>23</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" t="s" s="29">
+        <v>17</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" t="s" s="29">
+        <v>24</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" t="s" s="32">
+        <v>25</v>
       </c>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" t="s" s="9">
-        <v>24</v>
+      <c r="A5" t="s" s="29">
+        <v>26</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" t="s" s="29">
+        <v>17</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="E5" t="s" s="29">
+        <v>27</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="G5" t="s" s="32">
+        <v>28</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" t="s" s="7">
-        <v>25</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" t="s" s="9">
-        <v>27</v>
+      <c r="A6" t="s" s="29">
+        <v>29</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" t="s" s="29">
+        <v>17</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" t="s" s="29">
+        <v>30</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" t="s" s="32">
+        <v>31</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" t="s" s="9">
-        <v>30</v>
+      <c r="A7" t="s" s="29">
+        <v>32</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" t="s" s="29">
+        <v>17</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" t="s" s="29">
+        <v>33</v>
+      </c>
+      <c r="F7" s="31"/>
+      <c r="G7" t="s" s="32">
+        <v>34</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" t="s" s="9">
-        <v>33</v>
+      <c r="A8" t="s" s="29">
+        <v>35</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" t="s" s="29">
+        <v>17</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" t="s" s="29">
+        <v>36</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" t="s" s="32">
+        <v>37</v>
       </c>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" t="s" s="9">
-        <v>36</v>
+      <c r="A9" t="s" s="29">
+        <v>38</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" t="s" s="29">
+        <v>17</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" t="s" s="29">
+        <v>39</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" t="s" s="32">
+        <v>40</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" t="s" s="9">
-        <v>39</v>
+      <c r="A10" t="s" s="33">
+        <v>41</v>
+      </c>
+      <c r="B10" s="34"/>
+      <c r="C10" t="s" s="33">
+        <v>17</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" t="s" s="33">
+        <v>42</v>
+      </c>
+      <c r="F10" s="35"/>
+      <c r="G10" t="s" s="36">
+        <v>43</v>
       </c>
     </row>
     <row r="11" ht="16" customHeight="1">
-      <c r="A11" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" t="s" s="9">
-        <v>42</v>
+      <c r="A11" t="s" s="33">
+        <v>44</v>
+      </c>
+      <c r="B11" s="34"/>
+      <c r="C11" t="s" s="33">
+        <v>17</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" t="s" s="33">
+        <v>45</v>
+      </c>
+      <c r="F11" s="35"/>
+      <c r="G11" t="s" s="36">
+        <v>46</v>
       </c>
     </row>
     <row r="12" ht="16" customHeight="1">
-      <c r="A12" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="11"/>
+      <c r="A12" t="s" s="37">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s" s="37">
+        <v>17</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="40"/>
     </row>
     <row r="13" ht="16" customHeight="1">
-      <c r="A13" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="B13" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="11"/>
+      <c r="A13" t="s" s="37">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s" s="37">
+        <v>17</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="40"/>
     </row>
     <row r="14" ht="16" customHeight="1">
-      <c r="A14" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="B14" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="11"/>
+      <c r="A14" t="s" s="37">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s" s="37">
+        <v>17</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="40"/>
     </row>
     <row r="15" ht="16" customHeight="1">
-      <c r="A15" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="11"/>
+      <c r="A15" t="s" s="26">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2326,627 +2649,627 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="12" customWidth="1"/>
-    <col min="2" max="2" width="28.3516" style="12" customWidth="1"/>
-    <col min="3" max="8" width="8.85156" style="12" customWidth="1"/>
-    <col min="9" max="9" width="12.3516" style="12" customWidth="1"/>
-    <col min="10" max="10" width="29.5" style="12" customWidth="1"/>
-    <col min="11" max="11" width="8.85156" style="12" customWidth="1"/>
-    <col min="12" max="256" width="8.85156" style="12" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="43" customWidth="1"/>
+    <col min="2" max="2" width="28.3516" style="43" customWidth="1"/>
+    <col min="3" max="8" width="8.85156" style="43" customWidth="1"/>
+    <col min="9" max="9" width="12.3516" style="43" customWidth="1"/>
+    <col min="10" max="10" width="29.5" style="43" customWidth="1"/>
+    <col min="11" max="11" width="8.85156" style="43" customWidth="1"/>
+    <col min="12" max="256" width="8.85156" style="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="7">
+      <c r="A1" t="s" s="26">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s" s="26">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s" s="26">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s" s="26">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s" s="26">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s" s="26">
+        <v>54</v>
+      </c>
+      <c r="H1" s="44"/>
+      <c r="I1" s="42"/>
+      <c r="J1" t="s" s="28">
+        <v>55</v>
+      </c>
+      <c r="K1" s="42"/>
+    </row>
+    <row r="2" ht="16" customHeight="1">
+      <c r="A2" s="45">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="46">
+        <v>16</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" t="s" s="46">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s" s="46">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s" s="48">
+        <v>57</v>
+      </c>
+      <c r="I2" s="49"/>
+      <c r="J2" t="s" s="28">
+        <v>58</v>
+      </c>
+      <c r="K2" s="42"/>
+    </row>
+    <row r="3" ht="16" customHeight="1">
+      <c r="A3" s="45">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s" s="46">
+        <v>20</v>
+      </c>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" t="s" s="46">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s" s="46">
+        <v>56</v>
+      </c>
+      <c r="H3" s="50"/>
+      <c r="I3" t="s" s="51">
+        <v>59</v>
+      </c>
+      <c r="J3" t="s" s="52">
+        <v>60</v>
+      </c>
+      <c r="K3" t="s" s="28">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="45">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s" s="46">
+        <v>23</v>
+      </c>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" t="s" s="46">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s" s="46">
+        <v>56</v>
+      </c>
+      <c r="H4" s="50"/>
+      <c r="I4" s="53">
+        <v>0</v>
+      </c>
+      <c r="J4" s="54">
+        <v>0</v>
+      </c>
+      <c r="K4" s="55">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="45">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s" s="46">
+        <v>26</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" t="s" s="46">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s" s="46">
+        <v>56</v>
+      </c>
+      <c r="H5" s="50"/>
+      <c r="I5" s="53">
+        <v>1</v>
+      </c>
+      <c r="J5" s="54">
+        <v>1.5</v>
+      </c>
+      <c r="K5" s="55">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="45">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s" s="46">
+        <v>29</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" t="s" s="46">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s" s="46">
+        <v>56</v>
+      </c>
+      <c r="H6" s="50"/>
+      <c r="I6" s="53">
+        <v>2</v>
+      </c>
+      <c r="J6" s="54">
+        <v>3</v>
+      </c>
+      <c r="K6" s="55">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="45">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s" s="46">
+        <v>32</v>
+      </c>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" t="s" s="46">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s" s="46">
+        <v>56</v>
+      </c>
+      <c r="H7" s="50"/>
+      <c r="I7" s="53">
+        <v>3</v>
+      </c>
+      <c r="J7" s="54">
+        <v>3.5</v>
+      </c>
+      <c r="K7" s="55">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="45">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s" s="46">
+        <v>35</v>
+      </c>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" t="s" s="46">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s" s="46">
+        <v>56</v>
+      </c>
+      <c r="H8" s="50"/>
+      <c r="I8" s="53">
+        <v>4</v>
+      </c>
+      <c r="J8" s="54">
+        <v>4</v>
+      </c>
+      <c r="K8" s="55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="45">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s" s="46">
+        <v>38</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" t="s" s="46">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s" s="46">
+        <v>56</v>
+      </c>
+      <c r="H9" s="50"/>
+      <c r="I9" s="53">
+        <v>5</v>
+      </c>
+      <c r="J9" s="54">
+        <v>4.5</v>
+      </c>
+      <c r="K9" s="55">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" s="56">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s" s="57">
+        <v>41</v>
+      </c>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" t="s" s="57">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s" s="57">
+        <v>62</v>
+      </c>
+      <c r="H10" t="s" s="59">
+        <v>63</v>
+      </c>
+      <c r="I10" s="53">
+        <v>6</v>
+      </c>
+      <c r="J10" s="54">
+        <v>5</v>
+      </c>
+      <c r="K10" s="55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1">
+      <c r="A11" s="56">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s" s="57">
+        <v>44</v>
+      </c>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" t="s" s="57">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s" s="57">
+        <v>62</v>
+      </c>
+      <c r="H11" s="60"/>
+      <c r="I11" s="53">
+        <v>7</v>
+      </c>
+      <c r="J11" s="54">
+        <v>5.5</v>
+      </c>
+      <c r="K11" s="55">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1">
+      <c r="A12" s="41"/>
+      <c r="B12" t="s" s="26">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" t="s" s="61">
+        <v>64</v>
+      </c>
+      <c r="I12" s="62">
+        <v>8</v>
+      </c>
+      <c r="J12" s="54">
+        <v>6</v>
+      </c>
+      <c r="K12" s="55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1">
+      <c r="A13" s="41"/>
+      <c r="B13" t="s" s="26">
         <v>48</v>
       </c>
-      <c r="B1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s" s="7">
+      <c r="C13" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="62">
+        <v>9</v>
+      </c>
+      <c r="J13" s="54">
+        <v>6.5</v>
+      </c>
+      <c r="K13" s="55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1">
+      <c r="A14" s="41"/>
+      <c r="B14" t="s" s="26">
         <v>49</v>
       </c>
-      <c r="D1" t="s" s="7">
+      <c r="C14" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="62">
+        <v>10</v>
+      </c>
+      <c r="J14" s="54">
         <v>7</v>
       </c>
-      <c r="E1" t="s" s="7">
+      <c r="K14" s="55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" s="41"/>
+      <c r="B15" t="s" s="26">
         <v>50</v>
       </c>
-      <c r="F1" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s" s="7">
-        <v>51</v>
-      </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="11"/>
-      <c r="J1" t="s" s="9">
-        <v>52</v>
-      </c>
-      <c r="K1" s="11"/>
-    </row>
-    <row r="2" ht="16" customHeight="1">
-      <c r="A2" s="14">
+      <c r="C15" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" t="s" s="64">
+        <v>65</v>
+      </c>
+      <c r="I15" s="62">
+        <v>11</v>
+      </c>
+      <c r="J15" s="54"/>
+      <c r="K15" s="55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1">
+      <c r="A16" s="65"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="62">
+        <v>12</v>
+      </c>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" t="s" s="15">
+    </row>
+    <row r="17" ht="15" customHeight="1">
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="62">
         <v>13</v>
       </c>
-      <c r="G2" t="s" s="15">
-        <v>53</v>
-      </c>
-      <c r="H2" t="s" s="17">
-        <v>54</v>
-      </c>
-      <c r="I2" s="18"/>
-      <c r="J2" t="s" s="9">
-        <v>55</v>
-      </c>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="14">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s" s="15">
-        <v>16</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s" s="15">
-        <v>53</v>
-      </c>
-      <c r="H3" s="19"/>
-      <c r="I3" t="s" s="20">
-        <v>56</v>
-      </c>
-      <c r="J3" t="s" s="21">
-        <v>57</v>
-      </c>
-      <c r="K3" t="s" s="9">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="14">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s" s="15">
-        <v>19</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s" s="15">
-        <v>53</v>
-      </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="22">
+      <c r="J17" s="55"/>
+      <c r="K17" s="55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="62">
+        <v>14</v>
+      </c>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55">
         <v>0</v>
       </c>
-      <c r="J4" s="23">
-        <v>0</v>
-      </c>
-      <c r="K4" s="24">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="14">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s" s="15">
-        <v>22</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s" s="15">
-        <v>53</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="22">
-        <v>1</v>
-      </c>
-      <c r="J5" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="K5" s="24">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="14">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s" s="15">
-        <v>25</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s" s="15">
-        <v>53</v>
-      </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="22">
-        <v>2</v>
-      </c>
-      <c r="J6" s="23">
-        <v>3</v>
-      </c>
-      <c r="K6" s="24">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="14">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s" s="15">
-        <v>28</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s" s="15">
-        <v>53</v>
-      </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="22">
-        <v>3</v>
-      </c>
-      <c r="J7" s="23">
-        <v>3.5</v>
-      </c>
-      <c r="K7" s="24">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="14">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s" s="15">
-        <v>31</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s" s="15">
-        <v>53</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="22">
-        <v>4</v>
-      </c>
-      <c r="J8" s="23">
-        <v>4</v>
-      </c>
-      <c r="K8" s="24">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="14">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s" s="15">
-        <v>34</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s" s="15">
-        <v>53</v>
-      </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="22">
-        <v>5</v>
-      </c>
-      <c r="J9" s="23">
-        <v>4.5</v>
-      </c>
-      <c r="K9" s="24">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="25">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s" s="26">
-        <v>37</v>
-      </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" t="s" s="26">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s" s="26">
-        <v>59</v>
-      </c>
-      <c r="H10" t="s" s="28">
-        <v>60</v>
-      </c>
-      <c r="I10" s="22">
-        <v>6</v>
-      </c>
-      <c r="J10" s="23">
-        <v>5</v>
-      </c>
-      <c r="K10" s="24">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" s="25">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s" s="26">
-        <v>40</v>
-      </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" t="s" s="26">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s" s="26">
-        <v>59</v>
-      </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="22">
-        <v>7</v>
-      </c>
-      <c r="J11" s="23">
-        <v>5.5</v>
-      </c>
-      <c r="K11" s="24">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" t="s" s="30">
-        <v>61</v>
-      </c>
-      <c r="I12" s="31">
-        <v>8</v>
-      </c>
-      <c r="J12" s="23">
-        <v>6</v>
-      </c>
-      <c r="K12" s="24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C13" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="31">
-        <v>9</v>
-      </c>
-      <c r="J13" s="23">
-        <v>6.5</v>
-      </c>
-      <c r="K13" s="24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="C14" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="31">
-        <v>10</v>
-      </c>
-      <c r="J14" s="23">
-        <v>7</v>
-      </c>
-      <c r="K14" s="24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C15" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" t="s" s="33">
-        <v>62</v>
-      </c>
-      <c r="I15" s="31">
-        <v>11</v>
-      </c>
-      <c r="J15" s="23"/>
-      <c r="K15" s="24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="31">
-        <v>12</v>
-      </c>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" ht="15" customHeight="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="31">
-        <v>13</v>
-      </c>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="31">
-        <v>14</v>
-      </c>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24">
-        <v>0</v>
-      </c>
     </row>
     <row r="19" ht="15" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
     </row>
     <row r="20" ht="15" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
     </row>
     <row r="21" ht="15" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
     </row>
     <row r="22" ht="15" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
     </row>
     <row r="23" ht="15" customHeight="1">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
     </row>
     <row r="24" ht="15" customHeight="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
     </row>
     <row r="25" ht="15" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
     </row>
     <row r="26" ht="15" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
     </row>
     <row r="27" ht="15" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
     </row>
     <row r="28" ht="15" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
+      <c r="A28" s="42"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="42"/>
     </row>
     <row r="29" ht="15" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
     </row>
     <row r="30" ht="15" customHeight="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
     </row>
     <row r="31" ht="15" customHeight="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>